<commit_message>
Include balance of system in grid battery costs, unaffected by endogenous learning (#23)
</commit_message>
<xml_diff>
--- a/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
+++ b/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\elec\BCpUC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\elec\BCpUC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF11D8B-6961-42E1-8033-23B326896378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="2835" yWindow="1230" windowWidth="24765" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
-    <sheet name="Calculations" sheetId="1" r:id="rId2"/>
-    <sheet name="BCpUC" sheetId="3" r:id="rId3"/>
+    <sheet name="Battery Calculations" sheetId="1" r:id="rId2"/>
+    <sheet name="Balance of System Calculations" sheetId="5" r:id="rId3"/>
+    <sheet name="BCpUC" sheetId="3" r:id="rId4"/>
+    <sheet name="BBoSCpUC" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
   <si>
     <t>$/kW</t>
   </si>
@@ -123,9 +136,6 @@
   </si>
   <si>
     <t>See "cpi.xlsx" in the InputData folder for source information.</t>
-  </si>
-  <si>
-    <t>We adjust 2010 dollars to 2012 dollars using the following conversion factor:</t>
   </si>
   <si>
     <t>BCpUC Battery Cost per Unit Capacity</t>
@@ -183,15 +193,166 @@
   <si>
     <t>learning.</t>
   </si>
+  <si>
+    <t>BCpUC Battery Balance of System Cost per Unit Capacity</t>
+  </si>
+  <si>
+    <t>Unit: $/MW</t>
+  </si>
+  <si>
+    <t>Balance of System</t>
+  </si>
+  <si>
+    <t>Table 3. Detailed Cost Breakdown for a 60-MW U.S. Li-ion Standalone Storage System with Durations of 0.5–4 Hours</t>
+  </si>
+  <si>
+    <t>60-MW, 4-hour Duration, 240-MWh</t>
+  </si>
+  <si>
+    <t>60-MW, 2-hour Duration, 120-MWh</t>
+  </si>
+  <si>
+    <t>60-MW, 1-hour Duration, 60-MWh</t>
+  </si>
+  <si>
+    <t>60-MW, 0.5-hour Duration, 30-MWh</t>
+  </si>
+  <si>
+    <t>Li-ion battery</t>
+  </si>
+  <si>
+    <t>Battery central inverter</t>
+  </si>
+  <si>
+    <t>Structural BOS</t>
+  </si>
+  <si>
+    <t>Electrical BOS</t>
+  </si>
+  <si>
+    <t>EPC overhead</t>
+  </si>
+  <si>
+    <t>Sales tax</t>
+  </si>
+  <si>
+    <t>∑ EPC cost</t>
+  </si>
+  <si>
+    <t>Land acquisition</t>
+  </si>
+  <si>
+    <t>Permitting fee</t>
+  </si>
+  <si>
+    <t>Interconnection fee</t>
+  </si>
+  <si>
+    <t>Contingency</t>
+  </si>
+  <si>
+    <t>Developer overhead</t>
+  </si>
+  <si>
+    <t>EPC/developer net profit</t>
+  </si>
+  <si>
+    <t>∑ Developer cost</t>
+  </si>
+  <si>
+    <t>Total Cost ($)</t>
+  </si>
+  <si>
+    <t>$/W</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Model Component</t>
+  </si>
+  <si>
+    <t>Installation labor &amp; equipment</t>
+  </si>
+  <si>
+    <t>Balance of System Costs</t>
+  </si>
+  <si>
+    <t>https://www.nrel.gov/docs/fy19osti/71714.pdf</t>
+  </si>
+  <si>
+    <t>Page 12, Table 3</t>
+  </si>
+  <si>
+    <t>National Renewable Energy Laboratory</t>
+  </si>
+  <si>
+    <t>2018 U.S. Utility-Scale Photovoltaics Plus-Energy Storage System Costs Benchmark</t>
+  </si>
+  <si>
+    <t>Only the battery cost is affected by endogenous learning.  The "Balance of System"</t>
+  </si>
+  <si>
+    <t>costs are read directly from this variable and are not modified via endogenous learning</t>
+  </si>
+  <si>
+    <t>inside the simulator.</t>
+  </si>
+  <si>
+    <t>We use the largest (4-hour duration) for our estimate.</t>
+  </si>
+  <si>
+    <t>Balance of System (excl. sales tax)</t>
+  </si>
+  <si>
+    <t>Sales tax on balance of system elements</t>
+  </si>
+  <si>
+    <t>The "balance of system" should include all costs the utility must pay to purchase and</t>
+  </si>
+  <si>
+    <t>install the battery system, apart from the batteries themselves (and apart from sales</t>
+  </si>
+  <si>
+    <t>tax on the batteries).  This includes the inverter, labor, etc.</t>
+  </si>
+  <si>
+    <t>Currency Adjustment</t>
+  </si>
+  <si>
+    <t>2010 to 2012 USD</t>
+  </si>
+  <si>
+    <t>We adjust currency using the following conversion factors:</t>
+  </si>
+  <si>
+    <t>2018 $/W</t>
+  </si>
+  <si>
+    <t>2018 $/MW</t>
+  </si>
+  <si>
+    <t>2018 to 2012 USD</t>
+  </si>
+  <si>
+    <t>2012 $/MW</t>
+  </si>
+  <si>
+    <t>For the U.S. model, we assume the balance of system costs remain constant throughout the model run.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="#,##0;#,##0"/>
+    <numFmt numFmtId="170" formatCode="###0;###0"/>
+    <numFmt numFmtId="171" formatCode="###0.00;###0.00"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,8 +429,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,8 +464,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -333,6 +521,148 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -354,7 +684,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -383,16 +713,115 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="10" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
-    <cellStyle name="Footnotes: top row" xfId="7"/>
-    <cellStyle name="Header: bottom row" xfId="4"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6"/>
-    <cellStyle name="Table title" xfId="2"/>
+    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -427,7 +856,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -441,7 +869,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Calculations!$B$11</c:f>
+              <c:f>'Battery Calculations'!$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -474,7 +902,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>(Calculations!$A$16,Calculations!$A$18,Calculations!$A$20,Calculations!$A$22,Calculations!$A$24,Calculations!$A$26,Calculations!$A$28,Calculations!$A$30,Calculations!$A$32,Calculations!$A$34,Calculations!$A$36,Calculations!$A$38,Calculations!$A$40,Calculations!$A$42,Calculations!$A$44,Calculations!$A$46,Calculations!$A$48,Calculations!$A$50,Calculations!$A$52)</c:f>
+              <c:f>('Battery Calculations'!$A$16,'Battery Calculations'!$A$18,'Battery Calculations'!$A$20,'Battery Calculations'!$A$22,'Battery Calculations'!$A$24,'Battery Calculations'!$A$26,'Battery Calculations'!$A$28,'Battery Calculations'!$A$30,'Battery Calculations'!$A$32,'Battery Calculations'!$A$34,'Battery Calculations'!$A$36,'Battery Calculations'!$A$38,'Battery Calculations'!$A$40,'Battery Calculations'!$A$42,'Battery Calculations'!$A$44,'Battery Calculations'!$A$46,'Battery Calculations'!$A$48,'Battery Calculations'!$A$50,'Battery Calculations'!$A$52)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -540,7 +968,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>(Calculations!$B$16,Calculations!$B$18,Calculations!$B$20,Calculations!$B$22,Calculations!$B$24,Calculations!$B$26,Calculations!$B$28,Calculations!$B$30,Calculations!$B$32,Calculations!$B$34,Calculations!$B$36,Calculations!$B$38,Calculations!$B$40,Calculations!$B$42,Calculations!$B$44,Calculations!$B$46,Calculations!$B$48,Calculations!$B$50,Calculations!$B$52)</c:f>
+              <c:f>('Battery Calculations'!$B$16,'Battery Calculations'!$B$18,'Battery Calculations'!$B$20,'Battery Calculations'!$B$22,'Battery Calculations'!$B$24,'Battery Calculations'!$B$26,'Battery Calculations'!$B$28,'Battery Calculations'!$B$30,'Battery Calculations'!$B$32,'Battery Calculations'!$B$34,'Battery Calculations'!$B$36,'Battery Calculations'!$B$38,'Battery Calculations'!$B$40,'Battery Calculations'!$B$42,'Battery Calculations'!$B$44,'Battery Calculations'!$B$46,'Battery Calculations'!$B$48,'Battery Calculations'!$B$50,'Battery Calculations'!$B$52)</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
                 <c:ptCount val="19"/>
@@ -756,7 +1184,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -813,7 +1240,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1093,12 +1526,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1107,126 +1538,218 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="7">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
         <v>2014</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
         <v>2013</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+    <row r="17" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="26" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="28" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15">
+    <row r="29" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+    </row>
+    <row r="30" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+    </row>
+    <row r="35" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+    </row>
+    <row r="39" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
         <v>1.0549999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="59">
+        <v>0.9143273584567535</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B22" r:id="rId3" xr:uid="{CA93FE29-A0A0-406A-B94C-DC5006AB819F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1256,22 +1779,22 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1481,7 +2004,7 @@
         <v>135.565</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -1492,7 +2015,7 @@
         <v>133.44999999999999</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -1702,7 +2225,7 @@
         <v>2010</v>
       </c>
       <c r="C60" s="14">
-        <f>A60*About!$A$23</f>
+        <f>A60*About!$A$41</f>
         <v>636.16499999999996</v>
       </c>
     </row>
@@ -1714,7 +2237,7 @@
         <v>2010</v>
       </c>
       <c r="C61" s="14">
-        <f>A61*About!$A$23</f>
+        <f>A61*About!$A$41</f>
         <v>821.84499999999991</v>
       </c>
     </row>
@@ -1726,7 +2249,7 @@
         <v>2010</v>
       </c>
       <c r="C62" s="14">
-        <f>A62*About!$A$23</f>
+        <f>A62*About!$A$41</f>
         <v>750.1049999999999</v>
       </c>
     </row>
@@ -1738,7 +2261,7 @@
         <v>2010</v>
       </c>
       <c r="C63" s="14">
-        <f>A63*About!$A$23</f>
+        <f>A63*About!$A$41</f>
         <v>745.88499999999999</v>
       </c>
     </row>
@@ -1750,7 +2273,7 @@
         <v>2010</v>
       </c>
       <c r="C64" s="14">
-        <f>A64*About!$A$23</f>
+        <f>A64*About!$A$41</f>
         <v>672.03499999999997</v>
       </c>
     </row>
@@ -1785,7 +2308,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2350,11 +2873,802 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC34B27C-0BFA-4D35-874E-EA84BA74EBE0}">
+  <dimension ref="A1:M28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" style="20" customWidth="1"/>
+    <col min="2" max="13" width="11.28515625" style="20" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
+      <c r="B2" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="40"/>
+      <c r="M2" s="41"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="23">
+        <v>50160000</v>
+      </c>
+      <c r="C4" s="26">
+        <v>209</v>
+      </c>
+      <c r="D4" s="24">
+        <v>0.84</v>
+      </c>
+      <c r="E4" s="27">
+        <v>25080000</v>
+      </c>
+      <c r="F4" s="26">
+        <v>209</v>
+      </c>
+      <c r="G4" s="24">
+        <v>0.42</v>
+      </c>
+      <c r="H4" s="27">
+        <v>12540000</v>
+      </c>
+      <c r="I4" s="26">
+        <v>209</v>
+      </c>
+      <c r="J4" s="24">
+        <v>0.21</v>
+      </c>
+      <c r="K4" s="27">
+        <v>6270000</v>
+      </c>
+      <c r="L4" s="26">
+        <v>209</v>
+      </c>
+      <c r="M4" s="24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="23">
+        <v>4200000</v>
+      </c>
+      <c r="C5" s="26">
+        <v>18</v>
+      </c>
+      <c r="D5" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E5" s="27">
+        <v>4200000</v>
+      </c>
+      <c r="F5" s="26">
+        <v>35</v>
+      </c>
+      <c r="G5" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H5" s="27">
+        <v>4200000</v>
+      </c>
+      <c r="I5" s="26">
+        <v>70</v>
+      </c>
+      <c r="J5" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K5" s="27">
+        <v>4200000</v>
+      </c>
+      <c r="L5" s="26">
+        <v>140</v>
+      </c>
+      <c r="M5" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="23">
+        <v>3121131</v>
+      </c>
+      <c r="C6" s="26">
+        <v>13</v>
+      </c>
+      <c r="D6" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="E6" s="27">
+        <v>1813452</v>
+      </c>
+      <c r="F6" s="26">
+        <v>15</v>
+      </c>
+      <c r="G6" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="H6" s="27">
+        <v>1159612</v>
+      </c>
+      <c r="I6" s="26">
+        <v>19</v>
+      </c>
+      <c r="J6" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="K6" s="27">
+        <v>832692</v>
+      </c>
+      <c r="L6" s="26">
+        <v>28</v>
+      </c>
+      <c r="M6" s="24">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="23">
+        <v>8602825</v>
+      </c>
+      <c r="C7" s="26">
+        <v>36</v>
+      </c>
+      <c r="D7" s="24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E7" s="27">
+        <v>6119167</v>
+      </c>
+      <c r="F7" s="26">
+        <v>51</v>
+      </c>
+      <c r="G7" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="27">
+        <v>4877337</v>
+      </c>
+      <c r="I7" s="26">
+        <v>81</v>
+      </c>
+      <c r="J7" s="24">
+        <v>0.08</v>
+      </c>
+      <c r="K7" s="27">
+        <v>4256423</v>
+      </c>
+      <c r="L7" s="26">
+        <v>142</v>
+      </c>
+      <c r="M7" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="23">
+        <v>5479149</v>
+      </c>
+      <c r="C8" s="26">
+        <v>23</v>
+      </c>
+      <c r="D8" s="24">
+        <v>0.09</v>
+      </c>
+      <c r="E8" s="27">
+        <v>4322275</v>
+      </c>
+      <c r="F8" s="26">
+        <v>36</v>
+      </c>
+      <c r="G8" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H8" s="27">
+        <v>3743838</v>
+      </c>
+      <c r="I8" s="26">
+        <v>62</v>
+      </c>
+      <c r="J8" s="24">
+        <v>0.06</v>
+      </c>
+      <c r="K8" s="27">
+        <v>3454619</v>
+      </c>
+      <c r="L8" s="26">
+        <v>115</v>
+      </c>
+      <c r="M8" s="24">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="23">
+        <v>2775545</v>
+      </c>
+      <c r="C9" s="26">
+        <v>12</v>
+      </c>
+      <c r="D9" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="E9" s="27">
+        <v>1948565</v>
+      </c>
+      <c r="F9" s="26">
+        <v>16</v>
+      </c>
+      <c r="G9" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="H9" s="27">
+        <v>1535075</v>
+      </c>
+      <c r="I9" s="26">
+        <v>26</v>
+      </c>
+      <c r="J9" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="K9" s="27">
+        <v>1328330</v>
+      </c>
+      <c r="L9" s="26">
+        <v>44</v>
+      </c>
+      <c r="M9" s="24">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="23">
+        <v>5293460</v>
+      </c>
+      <c r="C10" s="26">
+        <v>22</v>
+      </c>
+      <c r="D10" s="24">
+        <v>0.09</v>
+      </c>
+      <c r="E10" s="27">
+        <v>3083292</v>
+      </c>
+      <c r="F10" s="26">
+        <v>26</v>
+      </c>
+      <c r="G10" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="H10" s="27">
+        <v>1978209</v>
+      </c>
+      <c r="I10" s="26">
+        <v>33</v>
+      </c>
+      <c r="J10" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="K10" s="27">
+        <v>1425667</v>
+      </c>
+      <c r="L10" s="26">
+        <v>48</v>
+      </c>
+      <c r="M10" s="24">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="43">
+        <v>79632110</v>
+      </c>
+      <c r="C11" s="44">
+        <v>332</v>
+      </c>
+      <c r="D11" s="45">
+        <v>1.33</v>
+      </c>
+      <c r="E11" s="46">
+        <v>46566751</v>
+      </c>
+      <c r="F11" s="44">
+        <v>388</v>
+      </c>
+      <c r="G11" s="45">
+        <v>0.78</v>
+      </c>
+      <c r="H11" s="46">
+        <v>30034071</v>
+      </c>
+      <c r="I11" s="44">
+        <v>501</v>
+      </c>
+      <c r="J11" s="45">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="46">
+        <v>21767732</v>
+      </c>
+      <c r="L11" s="44">
+        <v>726</v>
+      </c>
+      <c r="M11" s="45">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="21">
+        <v>250000</v>
+      </c>
+      <c r="C12" s="22">
+        <v>1</v>
+      </c>
+      <c r="D12" s="25">
+        <v>0</v>
+      </c>
+      <c r="E12" s="28">
+        <v>250000</v>
+      </c>
+      <c r="F12" s="22">
+        <v>2</v>
+      </c>
+      <c r="G12" s="25">
+        <v>0</v>
+      </c>
+      <c r="H12" s="28">
+        <v>250000</v>
+      </c>
+      <c r="I12" s="22">
+        <v>4</v>
+      </c>
+      <c r="J12" s="25">
+        <v>0</v>
+      </c>
+      <c r="K12" s="28">
+        <v>250000</v>
+      </c>
+      <c r="L12" s="22">
+        <v>8</v>
+      </c>
+      <c r="M12" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="23">
+        <v>295289</v>
+      </c>
+      <c r="C13" s="26">
+        <v>1</v>
+      </c>
+      <c r="D13" s="24">
+        <v>0</v>
+      </c>
+      <c r="E13" s="27">
+        <v>295289</v>
+      </c>
+      <c r="F13" s="26">
+        <v>2</v>
+      </c>
+      <c r="G13" s="24">
+        <v>0</v>
+      </c>
+      <c r="H13" s="27">
+        <v>295289</v>
+      </c>
+      <c r="I13" s="26">
+        <v>5</v>
+      </c>
+      <c r="J13" s="24">
+        <v>0</v>
+      </c>
+      <c r="K13" s="27">
+        <v>295289</v>
+      </c>
+      <c r="L13" s="26">
+        <v>10</v>
+      </c>
+      <c r="M13" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="23">
+        <v>1802363</v>
+      </c>
+      <c r="C14" s="26">
+        <v>8</v>
+      </c>
+      <c r="D14" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="E14" s="27">
+        <v>1802363</v>
+      </c>
+      <c r="F14" s="26">
+        <v>15</v>
+      </c>
+      <c r="G14" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="H14" s="27">
+        <v>1802363</v>
+      </c>
+      <c r="I14" s="26">
+        <v>30</v>
+      </c>
+      <c r="J14" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="K14" s="27">
+        <v>1802363</v>
+      </c>
+      <c r="L14" s="26">
+        <v>60</v>
+      </c>
+      <c r="M14" s="24">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="23">
+        <v>2477135</v>
+      </c>
+      <c r="C15" s="26">
+        <v>10</v>
+      </c>
+      <c r="D15" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="E15" s="27">
+        <v>1476303</v>
+      </c>
+      <c r="F15" s="26">
+        <v>12</v>
+      </c>
+      <c r="G15" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="H15" s="27">
+        <v>975887</v>
+      </c>
+      <c r="I15" s="26">
+        <v>16</v>
+      </c>
+      <c r="J15" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="K15" s="27">
+        <v>725679</v>
+      </c>
+      <c r="L15" s="26">
+        <v>24</v>
+      </c>
+      <c r="M15" s="24">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="23">
+        <v>2477135</v>
+      </c>
+      <c r="C16" s="26">
+        <v>10</v>
+      </c>
+      <c r="D16" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="E16" s="27">
+        <v>1476303</v>
+      </c>
+      <c r="F16" s="26">
+        <v>12</v>
+      </c>
+      <c r="G16" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="H16" s="27">
+        <v>975887</v>
+      </c>
+      <c r="I16" s="26">
+        <v>16</v>
+      </c>
+      <c r="J16" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="K16" s="27">
+        <v>725679</v>
+      </c>
+      <c r="L16" s="26">
+        <v>24</v>
+      </c>
+      <c r="M16" s="24">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="23">
+        <v>4346702</v>
+      </c>
+      <c r="C17" s="26">
+        <v>18</v>
+      </c>
+      <c r="D17" s="24">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E17" s="27">
+        <v>2593350</v>
+      </c>
+      <c r="F17" s="26">
+        <v>22</v>
+      </c>
+      <c r="G17" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="H17" s="27">
+        <v>1716675</v>
+      </c>
+      <c r="I17" s="26">
+        <v>29</v>
+      </c>
+      <c r="J17" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="K17" s="27">
+        <v>1278337</v>
+      </c>
+      <c r="L17" s="26">
+        <v>43</v>
+      </c>
+      <c r="M17" s="24">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="48">
+        <v>11648623</v>
+      </c>
+      <c r="C18" s="49">
+        <v>49</v>
+      </c>
+      <c r="D18" s="50">
+        <v>0.19</v>
+      </c>
+      <c r="E18" s="51">
+        <v>7893608</v>
+      </c>
+      <c r="F18" s="49">
+        <v>66</v>
+      </c>
+      <c r="G18" s="50">
+        <v>0.13</v>
+      </c>
+      <c r="H18" s="51">
+        <v>6016101</v>
+      </c>
+      <c r="I18" s="49">
+        <v>100</v>
+      </c>
+      <c r="J18" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="K18" s="51">
+        <v>5077347</v>
+      </c>
+      <c r="L18" s="49">
+        <v>169</v>
+      </c>
+      <c r="M18" s="50">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="55">
+        <f>SUM(D5:D9,D12:D17)</f>
+        <v>0.57999999999999985</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="57">
+        <f>D10*SUM(D5:D7)/SUM(D4:D7)</f>
+        <v>2.1272727272727273E-2</v>
+      </c>
+      <c r="E23" s="58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="55">
+        <f>SUM(D22:D23)</f>
+        <v>0.60127272727272707</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="60">
+        <f>D24*10^6</f>
+        <v>601272.72727272706</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="60">
+        <f>D25*About!A42</f>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="E26" s="58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF003399"/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2374,372 +3688,592 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>Calculations!A80</f>
-        <v>2014</v>
+        <f>'Battery Calculations'!A84</f>
+        <v>2018</v>
       </c>
       <c r="B2" s="9">
-        <f>Calculations!C80*1000</f>
-        <v>635681.28648150526</v>
+        <f>'Battery Calculations'!C84*1000</f>
+        <v>561998.2359458115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>Calculations!A81</f>
-        <v>2015</v>
+        <f>'Battery Calculations'!A85</f>
+        <v>2019</v>
       </c>
       <c r="B3" s="9">
-        <f>Calculations!C81*1000</f>
-        <v>615679.62000688352</v>
+        <f>'Battery Calculations'!C85*1000</f>
+        <v>545192.00172863714</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>Calculations!A82</f>
-        <v>2016</v>
+        <f>'Battery Calculations'!A86</f>
+        <v>2020</v>
       </c>
       <c r="B4" s="9">
-        <f>Calculations!C82*1000</f>
-        <v>596629.85829409957</v>
+        <f>'Battery Calculations'!C86*1000</f>
+        <v>528728.2359458115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>Calculations!A83</f>
-        <v>2017</v>
+        <f>'Battery Calculations'!A87</f>
+        <v>2021</v>
       </c>
       <c r="B5" s="9">
-        <f>Calculations!C83*1000</f>
-        <v>578532.00134338625</v>
+        <f>'Battery Calculations'!C87*1000</f>
+        <v>515659.62116147205</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>Calculations!A84</f>
-        <v>2018</v>
+        <f>'Battery Calculations'!A88</f>
+        <v>2022</v>
       </c>
       <c r="B6" s="9">
-        <f>Calculations!C84*1000</f>
-        <v>561998.2359458115</v>
+        <f>'Battery Calculations'!C88*1000</f>
+        <v>502568.2359458115</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>Calculations!A85</f>
-        <v>2019</v>
+        <f>'Battery Calculations'!A89</f>
+        <v>2023</v>
       </c>
       <c r="B7" s="9">
-        <f>Calculations!C85*1000</f>
-        <v>545192.00172863714</v>
+        <f>'Battery Calculations'!C89*1000</f>
+        <v>489934.8596421238</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>Calculations!A86</f>
-        <v>2020</v>
+        <f>'Battery Calculations'!A90</f>
+        <v>2024</v>
       </c>
       <c r="B8" s="9">
-        <f>Calculations!C86*1000</f>
-        <v>528728.2359458115</v>
+        <f>'Battery Calculations'!C90*1000</f>
+        <v>478998.23594581155</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>Calculations!A87</f>
-        <v>2021</v>
+        <f>'Battery Calculations'!A91</f>
+        <v>2025</v>
       </c>
       <c r="B9" s="9">
-        <f>Calculations!C87*1000</f>
-        <v>515659.62116147205</v>
+        <f>'Battery Calculations'!C91*1000</f>
+        <v>468017.71717082523</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>Calculations!A88</f>
-        <v>2022</v>
+        <f>'Battery Calculations'!A92</f>
+        <v>2026</v>
       </c>
       <c r="B10" s="9">
-        <f>Calculations!C88*1000</f>
-        <v>502568.2359458115</v>
+        <f>'Battery Calculations'!C92*1000</f>
+        <v>458538.2359458115</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>Calculations!A89</f>
-        <v>2023</v>
+        <f>'Battery Calculations'!A93</f>
+        <v>2027</v>
       </c>
       <c r="B11" s="9">
-        <f>Calculations!C89*1000</f>
-        <v>489934.8596421238</v>
+        <f>'Battery Calculations'!C93*1000</f>
+        <v>449908.19374757633</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>Calculations!A90</f>
-        <v>2024</v>
+        <f>'Battery Calculations'!A94</f>
+        <v>2028</v>
       </c>
       <c r="B12" s="9">
-        <f>Calculations!C90*1000</f>
-        <v>478998.23594581155</v>
+        <f>'Battery Calculations'!C94*1000</f>
+        <v>442128.23594581155</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>Calculations!A91</f>
-        <v>2025</v>
+        <f>'Battery Calculations'!A95</f>
+        <v>2029</v>
       </c>
       <c r="B13" s="9">
-        <f>Calculations!C91*1000</f>
-        <v>468017.71717082523</v>
+        <f>'Battery Calculations'!C95*1000</f>
+        <v>435606.2893723771</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>Calculations!A92</f>
-        <v>2026</v>
+        <f>'Battery Calculations'!A96</f>
+        <v>2030</v>
       </c>
       <c r="B14" s="9">
-        <f>Calculations!C92*1000</f>
-        <v>458538.2359458115</v>
+        <f>'Battery Calculations'!C96*1000</f>
+        <v>429848.2359458115</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f>Calculations!A93</f>
-        <v>2027</v>
+      <c r="A15" s="15">
+        <f>'Battery Calculations'!A97</f>
+        <v>2031</v>
       </c>
       <c r="B15" s="9">
-        <f>Calculations!C93*1000</f>
-        <v>449908.19374757633</v>
+        <f>'Battery Calculations'!C97*1000</f>
+        <v>427733.2359458115</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f>Calculations!A94</f>
-        <v>2028</v>
+      <c r="A16" s="15">
+        <f>'Battery Calculations'!A98</f>
+        <v>2032</v>
       </c>
       <c r="B16" s="9">
-        <f>Calculations!C94*1000</f>
-        <v>442128.23594581155</v>
+        <f>'Battery Calculations'!C98*1000</f>
+        <v>425618.2359458115</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f>Calculations!A95</f>
-        <v>2029</v>
+      <c r="A17" s="15">
+        <f>'Battery Calculations'!A99</f>
+        <v>2033</v>
       </c>
       <c r="B17" s="9">
-        <f>Calculations!C95*1000</f>
-        <v>435606.2893723771</v>
+        <f>'Battery Calculations'!C99*1000</f>
+        <v>424088.23594581144</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f>Calculations!A96</f>
-        <v>2030</v>
+      <c r="A18" s="15">
+        <f>'Battery Calculations'!A100</f>
+        <v>2034</v>
       </c>
       <c r="B18" s="9">
-        <f>Calculations!C96*1000</f>
-        <v>429848.2359458115</v>
+        <f>'Battery Calculations'!C100*1000</f>
+        <v>422558.2359458115</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
-        <f>Calculations!A97</f>
-        <v>2031</v>
+        <f>'Battery Calculations'!A101</f>
+        <v>2035</v>
       </c>
       <c r="B19" s="9">
-        <f>Calculations!C97*1000</f>
-        <v>427733.2359458115</v>
+        <f>'Battery Calculations'!C101*1000</f>
+        <v>421328.23594581144</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
-        <f>Calculations!A98</f>
-        <v>2032</v>
+        <f>'Battery Calculations'!A102</f>
+        <v>2036</v>
       </c>
       <c r="B20" s="9">
-        <f>Calculations!C98*1000</f>
-        <v>425618.2359458115</v>
+        <f>'Battery Calculations'!C102*1000</f>
+        <v>420098.2359458115</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
-        <f>Calculations!A99</f>
-        <v>2033</v>
+        <f>'Battery Calculations'!A103</f>
+        <v>2037</v>
       </c>
       <c r="B21" s="9">
-        <f>Calculations!C99*1000</f>
-        <v>424088.23594581144</v>
+        <f>'Battery Calculations'!C103*1000</f>
+        <v>419023.2359458115</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
-        <f>Calculations!A100</f>
-        <v>2034</v>
+        <f>'Battery Calculations'!A104</f>
+        <v>2038</v>
       </c>
       <c r="B22" s="9">
-        <f>Calculations!C100*1000</f>
-        <v>422558.2359458115</v>
+        <f>'Battery Calculations'!C104*1000</f>
+        <v>417948.23594581144</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
-        <f>Calculations!A101</f>
-        <v>2035</v>
+        <f>'Battery Calculations'!A105</f>
+        <v>2039</v>
       </c>
       <c r="B23" s="9">
-        <f>Calculations!C101*1000</f>
-        <v>421328.23594581144</v>
+        <f>'Battery Calculations'!C105*1000</f>
+        <v>416938.2359458115</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
-        <f>Calculations!A102</f>
-        <v>2036</v>
+        <f>'Battery Calculations'!A106</f>
+        <v>2040</v>
       </c>
       <c r="B24" s="9">
-        <f>Calculations!C102*1000</f>
-        <v>420098.2359458115</v>
+        <f>'Battery Calculations'!C106*1000</f>
+        <v>415928.2359458115</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
-        <f>Calculations!A103</f>
-        <v>2037</v>
+        <f>'Battery Calculations'!A107</f>
+        <v>2041</v>
       </c>
       <c r="B25" s="9">
-        <f>Calculations!C103*1000</f>
-        <v>419023.2359458115</v>
+        <f>'Battery Calculations'!C107*1000</f>
+        <v>414848.2359458115</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
-        <f>Calculations!A104</f>
-        <v>2038</v>
+        <f>'Battery Calculations'!A108</f>
+        <v>2042</v>
       </c>
       <c r="B26" s="9">
-        <f>Calculations!C104*1000</f>
-        <v>417948.23594581144</v>
+        <f>'Battery Calculations'!C108*1000</f>
+        <v>413768.2359458115</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
-        <f>Calculations!A105</f>
-        <v>2039</v>
+        <f>'Battery Calculations'!A109</f>
+        <v>2043</v>
       </c>
       <c r="B27" s="9">
-        <f>Calculations!C105*1000</f>
-        <v>416938.2359458115</v>
+        <f>'Battery Calculations'!C109*1000</f>
+        <v>412718.2359458115</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
-        <f>Calculations!A106</f>
-        <v>2040</v>
+        <f>'Battery Calculations'!A110</f>
+        <v>2044</v>
       </c>
       <c r="B28" s="9">
-        <f>Calculations!C106*1000</f>
-        <v>415928.2359458115</v>
+        <f>'Battery Calculations'!C110*1000</f>
+        <v>411668.2359458115</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
-        <f>Calculations!A107</f>
-        <v>2041</v>
+        <f>'Battery Calculations'!A111</f>
+        <v>2045</v>
       </c>
       <c r="B29" s="9">
-        <f>Calculations!C107*1000</f>
-        <v>414848.2359458115</v>
+        <f>'Battery Calculations'!C111*1000</f>
+        <v>410658.2359458115</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
-        <f>Calculations!A108</f>
-        <v>2042</v>
+        <f>'Battery Calculations'!A112</f>
+        <v>2046</v>
       </c>
       <c r="B30" s="9">
-        <f>Calculations!C108*1000</f>
-        <v>413768.2359458115</v>
+        <f>'Battery Calculations'!C112*1000</f>
+        <v>409648.2359458115</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
-        <f>Calculations!A109</f>
-        <v>2043</v>
+        <f>'Battery Calculations'!A113</f>
+        <v>2047</v>
       </c>
       <c r="B31" s="9">
-        <f>Calculations!C109*1000</f>
-        <v>412718.2359458115</v>
+        <f>'Battery Calculations'!C113*1000</f>
+        <v>408663.2359458115</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
-        <f>Calculations!A110</f>
-        <v>2044</v>
+        <f>'Battery Calculations'!A114</f>
+        <v>2048</v>
       </c>
       <c r="B32" s="9">
-        <f>Calculations!C110*1000</f>
-        <v>411668.2359458115</v>
+        <f>'Battery Calculations'!C114*1000</f>
+        <v>407678.2359458115</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
-        <f>Calculations!A111</f>
-        <v>2045</v>
+        <f>'Battery Calculations'!A115</f>
+        <v>2049</v>
       </c>
       <c r="B33" s="9">
-        <f>Calculations!C111*1000</f>
-        <v>410658.2359458115</v>
+        <f>'Battery Calculations'!C115*1000</f>
+        <v>406728.2359458115</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
-        <f>Calculations!A112</f>
+        <f>'Battery Calculations'!A116</f>
+        <v>2050</v>
+      </c>
+      <c r="B34" s="9">
+        <f>'Battery Calculations'!C116*1000</f>
+        <v>405778.2359458115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2600C7A-0160-47B2-B089-93F8CBD71882}">
+  <sheetPr>
+    <tabColor rgb="FF003399"/>
+  </sheetPr>
+  <dimension ref="A1:AH2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1">
+        <v>2018</v>
+      </c>
+      <c r="C1">
+        <v>2019</v>
+      </c>
+      <c r="D1" s="15">
+        <v>2020</v>
+      </c>
+      <c r="E1" s="15">
+        <v>2021</v>
+      </c>
+      <c r="F1" s="15">
+        <v>2022</v>
+      </c>
+      <c r="G1" s="15">
+        <v>2023</v>
+      </c>
+      <c r="H1" s="15">
+        <v>2024</v>
+      </c>
+      <c r="I1" s="15">
+        <v>2025</v>
+      </c>
+      <c r="J1" s="15">
+        <v>2026</v>
+      </c>
+      <c r="K1" s="15">
+        <v>2027</v>
+      </c>
+      <c r="L1" s="15">
+        <v>2028</v>
+      </c>
+      <c r="M1" s="15">
+        <v>2029</v>
+      </c>
+      <c r="N1" s="15">
+        <v>2030</v>
+      </c>
+      <c r="O1" s="15">
+        <v>2031</v>
+      </c>
+      <c r="P1" s="15">
+        <v>2032</v>
+      </c>
+      <c r="Q1" s="15">
+        <v>2033</v>
+      </c>
+      <c r="R1" s="15">
+        <v>2034</v>
+      </c>
+      <c r="S1" s="15">
+        <v>2035</v>
+      </c>
+      <c r="T1" s="15">
+        <v>2036</v>
+      </c>
+      <c r="U1" s="15">
+        <v>2037</v>
+      </c>
+      <c r="V1" s="15">
+        <v>2038</v>
+      </c>
+      <c r="W1" s="15">
+        <v>2039</v>
+      </c>
+      <c r="X1" s="15">
+        <v>2040</v>
+      </c>
+      <c r="Y1" s="15">
+        <v>2041</v>
+      </c>
+      <c r="Z1" s="15">
+        <v>2042</v>
+      </c>
+      <c r="AA1" s="15">
+        <v>2043</v>
+      </c>
+      <c r="AB1" s="15">
+        <v>2044</v>
+      </c>
+      <c r="AC1" s="15">
+        <v>2045</v>
+      </c>
+      <c r="AD1" s="15">
         <v>2046</v>
       </c>
-      <c r="B34" s="9">
-        <f>Calculations!C112*1000</f>
-        <v>409648.2359458115</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
-        <f>Calculations!A113</f>
+      <c r="AE1" s="15">
         <v>2047</v>
       </c>
-      <c r="B35" s="9">
-        <f>Calculations!C113*1000</f>
-        <v>408663.2359458115</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
-        <f>Calculations!A114</f>
+      <c r="AF1" s="15">
         <v>2048</v>
       </c>
-      <c r="B36" s="9">
-        <f>Calculations!C114*1000</f>
-        <v>407678.2359458115</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
-        <f>Calculations!A115</f>
+      <c r="AG1" s="15">
         <v>2049</v>
       </c>
-      <c r="B37" s="9">
-        <f>Calculations!C115*1000</f>
-        <v>406728.2359458115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
-        <f>Calculations!A116</f>
+      <c r="AH1" s="15">
         <v>2050</v>
       </c>
-      <c r="B38" s="9">
-        <f>Calculations!C116*1000</f>
-        <v>405778.2359458115</v>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="9">
+        <f>'Balance of System Calculations'!D26</f>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="C2" s="9">
+        <f>$B2</f>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="D2" s="9">
+        <f t="shared" ref="D2:AH2" si="0">$B2</f>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="E2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="F2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="G2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="H2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="I2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="J2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="K2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="L2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="M2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="N2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="O2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="P2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="Q2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="R2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="S2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="T2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="U2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="V2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="W2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="X2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="Y2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="Z2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AA2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AB2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AC2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AD2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AE2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AF2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AG2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
+      </c>
+      <c r="AH2" s="9">
+        <f t="shared" si="0"/>
+        <v>549760.10443936056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update expiration year for elec sector IRA tax credits
</commit_message>
<xml_diff>
--- a/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
+++ b/InputData/elec/BCpUC/Battery Cost per Unit Cap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\BCpUC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999D7867-60B9-40C5-9EDF-D7A44AA77B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F6D865-6970-43AC-AAE4-3A52F19D49FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="839" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -505,13 +505,13 @@
     <t>Raw Data (2022 $)</t>
   </si>
   <si>
-    <t>Battery Power Cost per Unit Capacity : NDC</t>
-  </si>
-  <si>
     <t>Time (Year)</t>
   </si>
   <si>
-    <t>Battery Energy Cost per Unit Capacity : NDC</t>
+    <t>Battery Energy Cost per Unit Capacity : MostRecentRun</t>
+  </si>
+  <si>
+    <t>Battery Power Cost per Unit Capacity : MostRecentRun</t>
   </si>
 </sst>
 </file>
@@ -1968,69 +1968,15 @@
     <xf numFmtId="5" fontId="10" fillId="14" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="10" fillId="14" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -2077,6 +2023,60 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="63" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2224,85 +2224,85 @@
                   <c:v>303546</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>277345</c:v>
+                  <c:v>275720</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>256728</c:v>
+                  <c:v>254008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>240275</c:v>
+                  <c:v>237399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>226464</c:v>
+                  <c:v>223663</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>214618</c:v>
+                  <c:v>212018</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>204553</c:v>
+                  <c:v>202332</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>196075</c:v>
+                  <c:v>194107</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>188655</c:v>
+                  <c:v>186872</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>182183</c:v>
+                  <c:v>180500</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>176401</c:v>
+                  <c:v>174745</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>171611</c:v>
+                  <c:v>169959</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>167430</c:v>
+                  <c:v>165780</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>163809</c:v>
+                  <c:v>162166</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>160633</c:v>
+                  <c:v>159002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>157780</c:v>
+                  <c:v>156172</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>155218</c:v>
+                  <c:v>153632</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>152921</c:v>
+                  <c:v>151363</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>150890</c:v>
+                  <c:v>149361</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>149018</c:v>
+                  <c:v>147535</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>147310</c:v>
+                  <c:v>145853</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>145744</c:v>
+                  <c:v>144309</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>144287</c:v>
+                  <c:v>142883</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>142963</c:v>
+                  <c:v>141583</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>141726</c:v>
+                  <c:v>140367</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>140576</c:v>
+                  <c:v>139237</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>139495</c:v>
+                  <c:v>138175</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>138485</c:v>
+                  <c:v>137182</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4911,19 +4911,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:108" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="142" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="165"/>
-      <c r="K1" s="165"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
       <c r="M1" s="3" t="s">
         <v>68</v>
       </c>
@@ -5053,12 +5053,12 @@
     </row>
     <row r="4" spans="1:108" s="40" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="44"/>
-      <c r="L4" s="166" t="s">
+      <c r="L4" s="143" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:108" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L5" s="167"/>
+      <c r="L5" s="144"/>
     </row>
     <row r="6" spans="1:108" s="40" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H6" s="45"/>
@@ -5090,23 +5090,23 @@
       <c r="B7" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="161" t="s">
+      <c r="C7" s="145" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="161"/>
-      <c r="E7" s="161"/>
-      <c r="F7" s="161"/>
-      <c r="G7" s="161"/>
-      <c r="H7" s="161"/>
-      <c r="I7" s="161"/>
-      <c r="J7" s="161"/>
-      <c r="K7" s="161"/>
-      <c r="L7" s="161"/>
-      <c r="M7" s="161"/>
-      <c r="N7" s="161"/>
-      <c r="O7" s="161"/>
-      <c r="P7" s="161"/>
-      <c r="Q7" s="161"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="145"/>
+      <c r="F7" s="145"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
+      <c r="K7" s="145"/>
+      <c r="L7" s="145"/>
+      <c r="M7" s="145"/>
+      <c r="N7" s="145"/>
+      <c r="O7" s="145"/>
+      <c r="P7" s="145"/>
+      <c r="Q7" s="145"/>
       <c r="R7" s="50"/>
       <c r="S7" s="50"/>
       <c r="T7" s="50"/>
@@ -5124,43 +5124,43 @@
     </row>
     <row r="9" spans="1:108" s="40" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9"/>
-      <c r="B9" s="168" t="s">
+      <c r="B9" s="146" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="169" t="s">
+      <c r="D9" s="147" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="170"/>
-      <c r="F9" s="171"/>
-      <c r="G9" s="172">
+      <c r="E9" s="148"/>
+      <c r="F9" s="149"/>
+      <c r="G9" s="150">
         <v>2021</v>
       </c>
-      <c r="H9" s="173"/>
-      <c r="I9" s="173"/>
-      <c r="J9" s="173"/>
-      <c r="K9" s="174"/>
-      <c r="L9" s="174"/>
+      <c r="H9" s="151"/>
+      <c r="I9" s="151"/>
+      <c r="J9" s="151"/>
+      <c r="K9" s="152"/>
+      <c r="L9" s="152"/>
     </row>
     <row r="10" spans="1:108" s="40" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="168"/>
+      <c r="B10" s="146"/>
       <c r="D10" s="53" t="s">
         <v>76</v>
       </c>
       <c r="J10" s="52"/>
     </row>
     <row r="11" spans="1:108" s="40" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="168"/>
-      <c r="D11" s="175" t="s">
+      <c r="B11" s="146"/>
+      <c r="D11" s="153" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="176"/>
-      <c r="F11" s="176"/>
-      <c r="G11" s="176"/>
-      <c r="H11" s="176"/>
-      <c r="I11" s="176"/>
-      <c r="J11" s="176"/>
-      <c r="K11" s="176"/>
-      <c r="L11" s="176"/>
+      <c r="E11" s="154"/>
+      <c r="F11" s="154"/>
+      <c r="G11" s="154"/>
+      <c r="H11" s="154"/>
+      <c r="I11" s="154"/>
+      <c r="J11" s="154"/>
+      <c r="K11" s="154"/>
+      <c r="L11" s="154"/>
       <c r="W11" s="54"/>
       <c r="X11" s="55"/>
       <c r="Y11" s="55"/>
@@ -5168,18 +5168,18 @@
       <c r="AA11" s="55"/>
     </row>
     <row r="12" spans="1:108" s="40" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="168"/>
-      <c r="D12" s="177" t="s">
+      <c r="B12" s="146"/>
+      <c r="D12" s="155" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="178"/>
-      <c r="F12" s="178"/>
-      <c r="G12" s="178"/>
-      <c r="H12" s="178"/>
-      <c r="I12" s="178"/>
-      <c r="J12" s="178"/>
-      <c r="K12" s="178"/>
-      <c r="L12" s="179"/>
+      <c r="E12" s="156"/>
+      <c r="F12" s="156"/>
+      <c r="G12" s="156"/>
+      <c r="H12" s="156"/>
+      <c r="I12" s="156"/>
+      <c r="J12" s="156"/>
+      <c r="K12" s="156"/>
+      <c r="L12" s="157"/>
       <c r="M12" s="56"/>
       <c r="W12" s="54"/>
       <c r="X12" s="55"/>
@@ -5188,16 +5188,16 @@
       <c r="AA12" s="55"/>
     </row>
     <row r="13" spans="1:108" s="40" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="168"/>
-      <c r="D13" s="180"/>
-      <c r="E13" s="181"/>
-      <c r="F13" s="181"/>
-      <c r="G13" s="181"/>
-      <c r="H13" s="181"/>
-      <c r="I13" s="181"/>
-      <c r="J13" s="181"/>
-      <c r="K13" s="181"/>
-      <c r="L13" s="182"/>
+      <c r="B13" s="146"/>
+      <c r="D13" s="158"/>
+      <c r="E13" s="159"/>
+      <c r="F13" s="159"/>
+      <c r="G13" s="159"/>
+      <c r="H13" s="159"/>
+      <c r="I13" s="159"/>
+      <c r="J13" s="159"/>
+      <c r="K13" s="159"/>
+      <c r="L13" s="160"/>
       <c r="W13" s="54"/>
       <c r="X13" s="55"/>
       <c r="Y13" s="55"/>
@@ -5205,49 +5205,49 @@
       <c r="AA13" s="55"/>
     </row>
     <row r="14" spans="1:108" ht="37.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="168"/>
+      <c r="B14" s="146"/>
     </row>
     <row r="15" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="B15" s="168"/>
-      <c r="C15" s="183" t="s">
+      <c r="B15" s="146"/>
+      <c r="C15" s="161" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="183"/>
-      <c r="E15" s="183"/>
-      <c r="F15" s="183"/>
-      <c r="G15" s="183"/>
-      <c r="H15" s="183"/>
-      <c r="I15" s="183"/>
-      <c r="J15" s="183"/>
-      <c r="K15" s="183"/>
-      <c r="L15" s="183"/>
-      <c r="M15" s="183"/>
-      <c r="N15" s="183"/>
-      <c r="O15" s="183"/>
-      <c r="P15" s="183"/>
+      <c r="D15" s="161"/>
+      <c r="E15" s="161"/>
+      <c r="F15" s="161"/>
+      <c r="G15" s="161"/>
+      <c r="H15" s="161"/>
+      <c r="I15" s="161"/>
+      <c r="J15" s="161"/>
+      <c r="K15" s="161"/>
+      <c r="L15" s="161"/>
+      <c r="M15" s="161"/>
+      <c r="N15" s="161"/>
+      <c r="O15" s="161"/>
+      <c r="P15" s="161"/>
       <c r="Q15" s="57"/>
     </row>
     <row r="16" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="B16" s="168"/>
-      <c r="C16" s="183"/>
-      <c r="D16" s="183"/>
-      <c r="E16" s="183"/>
-      <c r="F16" s="183"/>
-      <c r="G16" s="183"/>
-      <c r="H16" s="183"/>
-      <c r="I16" s="183"/>
-      <c r="J16" s="183"/>
-      <c r="K16" s="183"/>
-      <c r="L16" s="183"/>
-      <c r="M16" s="183"/>
-      <c r="N16" s="183"/>
-      <c r="O16" s="183"/>
-      <c r="P16" s="183"/>
+      <c r="B16" s="146"/>
+      <c r="C16" s="161"/>
+      <c r="D16" s="161"/>
+      <c r="E16" s="161"/>
+      <c r="F16" s="161"/>
+      <c r="G16" s="161"/>
+      <c r="H16" s="161"/>
+      <c r="I16" s="161"/>
+      <c r="J16" s="161"/>
+      <c r="K16" s="161"/>
+      <c r="L16" s="161"/>
+      <c r="M16" s="161"/>
+      <c r="N16" s="161"/>
+      <c r="O16" s="161"/>
+      <c r="P16" s="161"/>
     </row>
     <row r="17" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="168"/>
+      <c r="B17" s="146"/>
       <c r="C17" s="58"/>
-      <c r="D17" s="158" t="s">
+      <c r="D17" s="168" t="s">
         <v>80</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -5255,9 +5255,9 @@
       </c>
     </row>
     <row r="18" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="168"/>
+      <c r="B18" s="146"/>
       <c r="C18" s="58"/>
-      <c r="D18" s="159"/>
+      <c r="D18" s="169"/>
       <c r="F18" s="1">
         <v>2021</v>
       </c>
@@ -5350,9 +5350,9 @@
       </c>
     </row>
     <row r="19" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="168"/>
+      <c r="B19" s="146"/>
       <c r="C19" s="58"/>
-      <c r="D19" s="159"/>
+      <c r="D19" s="169"/>
       <c r="E19" t="s">
         <v>82</v>
       </c>
@@ -5448,9 +5448,9 @@
       </c>
     </row>
     <row r="20" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="168"/>
+      <c r="B20" s="146"/>
       <c r="C20" s="58"/>
-      <c r="D20" s="160"/>
+      <c r="D20" s="170"/>
       <c r="E20" t="s">
         <v>83</v>
       </c>
@@ -5546,9 +5546,9 @@
       </c>
     </row>
     <row r="21" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="168"/>
+      <c r="B21" s="146"/>
       <c r="C21" s="58"/>
-      <c r="D21" s="160"/>
+      <c r="D21" s="170"/>
       <c r="E21" t="s">
         <v>84</v>
       </c>
@@ -5644,9 +5644,9 @@
       </c>
     </row>
     <row r="22" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="168"/>
+      <c r="B22" s="146"/>
       <c r="C22" s="58"/>
-      <c r="D22" s="160"/>
+      <c r="D22" s="170"/>
       <c r="F22" s="60"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -5679,18 +5679,18 @@
       <c r="AI22" s="5"/>
     </row>
     <row r="23" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="168"/>
+      <c r="B23" s="146"/>
       <c r="C23" s="58"/>
-      <c r="D23" s="160"/>
+      <c r="D23" s="170"/>
       <c r="E23" s="1" t="s">
         <v>85</v>
       </c>
       <c r="F23" s="60"/>
     </row>
     <row r="24" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="168"/>
+      <c r="B24" s="146"/>
       <c r="C24" s="58"/>
-      <c r="D24" s="160"/>
+      <c r="D24" s="170"/>
       <c r="F24" s="1">
         <v>2021</v>
       </c>
@@ -5783,9 +5783,9 @@
       </c>
     </row>
     <row r="25" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="168"/>
+      <c r="B25" s="146"/>
       <c r="C25" s="58"/>
-      <c r="D25" s="160"/>
+      <c r="D25" s="170"/>
       <c r="E25" t="s">
         <v>82</v>
       </c>
@@ -5881,9 +5881,9 @@
       </c>
     </row>
     <row r="26" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="168"/>
+      <c r="B26" s="146"/>
       <c r="C26" s="58"/>
-      <c r="D26" s="160"/>
+      <c r="D26" s="170"/>
       <c r="E26" t="s">
         <v>83</v>
       </c>
@@ -5979,9 +5979,9 @@
       </c>
     </row>
     <row r="27" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="168"/>
+      <c r="B27" s="146"/>
       <c r="C27" s="58"/>
-      <c r="D27" s="160"/>
+      <c r="D27" s="170"/>
       <c r="E27" t="s">
         <v>84</v>
       </c>
@@ -6077,7 +6077,7 @@
       </c>
     </row>
     <row r="28" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="168"/>
+      <c r="B28" s="146"/>
       <c r="C28" s="58"/>
       <c r="D28" s="58"/>
       <c r="G28" s="5"/>
@@ -6115,7 +6115,7 @@
       <c r="AM28" s="5"/>
     </row>
     <row r="29" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="168"/>
+      <c r="B29" s="146"/>
       <c r="C29" s="58"/>
       <c r="D29" s="58"/>
       <c r="E29" s="1" t="s">
@@ -6157,7 +6157,7 @@
       <c r="AM29" s="5"/>
     </row>
     <row r="30" spans="2:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="168"/>
+      <c r="B30" s="146"/>
       <c r="C30" s="58"/>
       <c r="D30" s="58"/>
       <c r="E30" s="1"/>
@@ -6197,9 +6197,9 @@
       <c r="AM30" s="5"/>
     </row>
     <row r="31" spans="2:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="168"/>
+      <c r="B31" s="146"/>
       <c r="C31" s="58"/>
-      <c r="D31" s="159" t="s">
+      <c r="D31" s="169" t="s">
         <v>87</v>
       </c>
       <c r="E31" s="61" t="s">
@@ -6249,9 +6249,9 @@
       <c r="AM31" s="5"/>
     </row>
     <row r="32" spans="2:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="168"/>
+      <c r="B32" s="146"/>
       <c r="C32" s="58"/>
-      <c r="D32" s="159"/>
+      <c r="D32" s="169"/>
       <c r="E32" s="66" t="s">
         <v>93</v>
       </c>
@@ -6299,9 +6299,9 @@
       <c r="AM32" s="5"/>
     </row>
     <row r="33" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="168"/>
+      <c r="B33" s="146"/>
       <c r="C33" s="58"/>
-      <c r="D33" s="159"/>
+      <c r="D33" s="169"/>
       <c r="E33" s="69" t="s">
         <v>98</v>
       </c>
@@ -6349,9 +6349,9 @@
       <c r="AM33" s="5"/>
     </row>
     <row r="34" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="168"/>
+      <c r="B34" s="146"/>
       <c r="C34" s="58"/>
-      <c r="D34" s="159"/>
+      <c r="D34" s="169"/>
       <c r="E34" s="72" t="s">
         <v>100</v>
       </c>
@@ -6399,9 +6399,9 @@
       <c r="AM34" s="5"/>
     </row>
     <row r="35" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="168"/>
+      <c r="B35" s="146"/>
       <c r="C35" s="58"/>
-      <c r="D35" s="159"/>
+      <c r="D35" s="169"/>
       <c r="E35" s="69" t="s">
         <v>102</v>
       </c>
@@ -6449,9 +6449,9 @@
       <c r="AM35" s="5"/>
     </row>
     <row r="36" spans="2:74" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="168"/>
+      <c r="B36" s="146"/>
       <c r="C36" s="58"/>
-      <c r="D36" s="159"/>
+      <c r="D36" s="169"/>
       <c r="E36" s="75" t="s">
         <v>104</v>
       </c>
@@ -6538,23 +6538,23 @@
       <c r="AM37" s="5"/>
     </row>
     <row r="38" spans="2:74" s="40" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="161" t="s">
+      <c r="C38" s="145" t="s">
         <v>106</v>
       </c>
-      <c r="D38" s="161"/>
-      <c r="E38" s="161"/>
-      <c r="F38" s="161"/>
-      <c r="G38" s="161"/>
-      <c r="H38" s="161"/>
-      <c r="I38" s="161"/>
-      <c r="J38" s="161"/>
-      <c r="K38" s="161"/>
-      <c r="L38" s="161"/>
-      <c r="M38" s="161"/>
-      <c r="N38" s="161"/>
-      <c r="O38" s="161"/>
-      <c r="P38" s="161"/>
-      <c r="Q38" s="161"/>
+      <c r="D38" s="145"/>
+      <c r="E38" s="145"/>
+      <c r="F38" s="145"/>
+      <c r="G38" s="145"/>
+      <c r="H38" s="145"/>
+      <c r="I38" s="145"/>
+      <c r="J38" s="145"/>
+      <c r="K38" s="145"/>
+      <c r="L38" s="145"/>
+      <c r="M38" s="145"/>
+      <c r="N38" s="145"/>
+      <c r="O38" s="145"/>
+      <c r="P38" s="145"/>
+      <c r="Q38" s="145"/>
       <c r="R38" s="50"/>
       <c r="S38" s="50"/>
       <c r="T38" s="50"/>
@@ -6687,10 +6687,10 @@
       </c>
     </row>
     <row r="43" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="163" t="s">
+      <c r="B43" s="177" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="158" t="s">
+      <c r="D43" s="168" t="s">
         <v>109</v>
       </c>
       <c r="E43" s="79" t="s">
@@ -6792,8 +6792,8 @@
       </c>
     </row>
     <row r="44" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B44" s="163"/>
-      <c r="D44" s="159"/>
+      <c r="B44" s="177"/>
+      <c r="D44" s="169"/>
       <c r="E44" s="82" t="s">
         <v>93</v>
       </c>
@@ -6893,8 +6893,8 @@
       </c>
     </row>
     <row r="45" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B45" s="163"/>
-      <c r="D45" s="159"/>
+      <c r="B45" s="177"/>
+      <c r="D45" s="169"/>
       <c r="E45" s="83" t="s">
         <v>93</v>
       </c>
@@ -6994,8 +6994,8 @@
       </c>
     </row>
     <row r="46" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B46" s="163"/>
-      <c r="D46" s="160"/>
+      <c r="B46" s="177"/>
+      <c r="D46" s="170"/>
       <c r="E46" s="79" t="s">
         <v>98</v>
       </c>
@@ -7128,8 +7128,8 @@
       <c r="BV46" s="5"/>
     </row>
     <row r="47" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B47" s="163"/>
-      <c r="D47" s="160"/>
+      <c r="B47" s="177"/>
+      <c r="D47" s="170"/>
       <c r="E47" s="79" t="s">
         <v>98</v>
       </c>
@@ -7262,8 +7262,8 @@
       <c r="BV47" s="5"/>
     </row>
     <row r="48" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B48" s="163"/>
-      <c r="D48" s="160"/>
+      <c r="B48" s="177"/>
+      <c r="D48" s="170"/>
       <c r="E48" s="79" t="s">
         <v>98</v>
       </c>
@@ -7396,8 +7396,8 @@
       <c r="BV48" s="5"/>
     </row>
     <row r="49" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B49" s="163"/>
-      <c r="D49" s="160"/>
+      <c r="B49" s="177"/>
+      <c r="D49" s="170"/>
       <c r="E49" s="79" t="s">
         <v>100</v>
       </c>
@@ -7530,8 +7530,8 @@
       <c r="BV49" s="5"/>
     </row>
     <row r="50" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B50" s="163"/>
-      <c r="D50" s="160"/>
+      <c r="B50" s="177"/>
+      <c r="D50" s="170"/>
       <c r="E50" s="79" t="s">
         <v>100</v>
       </c>
@@ -7664,8 +7664,8 @@
       <c r="BV50" s="5"/>
     </row>
     <row r="51" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B51" s="163"/>
-      <c r="D51" s="160"/>
+      <c r="B51" s="177"/>
+      <c r="D51" s="170"/>
       <c r="E51" s="79" t="s">
         <v>100</v>
       </c>
@@ -7798,8 +7798,8 @@
       <c r="BV51" s="5"/>
     </row>
     <row r="52" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B52" s="163"/>
-      <c r="D52" s="160"/>
+      <c r="B52" s="177"/>
+      <c r="D52" s="170"/>
       <c r="E52" s="79" t="s">
         <v>102</v>
       </c>
@@ -7932,8 +7932,8 @@
       <c r="BV52" s="5"/>
     </row>
     <row r="53" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B53" s="163"/>
-      <c r="D53" s="160"/>
+      <c r="B53" s="177"/>
+      <c r="D53" s="170"/>
       <c r="E53" s="79" t="s">
         <v>102</v>
       </c>
@@ -8066,8 +8066,8 @@
       <c r="BV53" s="5"/>
     </row>
     <row r="54" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B54" s="163"/>
-      <c r="D54" s="160"/>
+      <c r="B54" s="177"/>
+      <c r="D54" s="170"/>
       <c r="E54" s="79" t="s">
         <v>102</v>
       </c>
@@ -8200,8 +8200,8 @@
       <c r="BV54" s="5"/>
     </row>
     <row r="55" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B55" s="163"/>
-      <c r="D55" s="160"/>
+      <c r="B55" s="177"/>
+      <c r="D55" s="170"/>
       <c r="E55" s="79" t="s">
         <v>104</v>
       </c>
@@ -8334,8 +8334,8 @@
       <c r="BV55" s="5"/>
     </row>
     <row r="56" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B56" s="163"/>
-      <c r="D56" s="160"/>
+      <c r="B56" s="177"/>
+      <c r="D56" s="170"/>
       <c r="E56" s="79" t="s">
         <v>104</v>
       </c>
@@ -8468,8 +8468,8 @@
       <c r="BV56" s="5"/>
     </row>
     <row r="57" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B57" s="163"/>
-      <c r="D57" s="160"/>
+      <c r="B57" s="177"/>
+      <c r="D57" s="170"/>
       <c r="E57" s="79" t="s">
         <v>104</v>
       </c>
@@ -8602,7 +8602,7 @@
       <c r="BV57" s="5"/>
     </row>
     <row r="58" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B58" s="163"/>
+      <c r="B58" s="177"/>
       <c r="D58" s="58"/>
       <c r="E58" s="82"/>
       <c r="F58" s="82"/>
@@ -8671,7 +8671,7 @@
       <c r="BV58" s="5"/>
     </row>
     <row r="59" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B59" s="163"/>
+      <c r="B59" s="177"/>
       <c r="D59" s="58"/>
       <c r="E59" s="82"/>
       <c r="F59" s="82"/>
@@ -8740,7 +8740,7 @@
       <c r="BV59" s="5"/>
     </row>
     <row r="60" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B60" s="163"/>
+      <c r="B60" s="177"/>
       <c r="D60" s="58"/>
       <c r="E60" s="82"/>
       <c r="F60" s="82"/>
@@ -8809,7 +8809,7 @@
       <c r="BV60" s="5"/>
     </row>
     <row r="61" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B61" s="163"/>
+      <c r="B61" s="177"/>
       <c r="D61" s="84"/>
       <c r="E61" s="82"/>
       <c r="F61" s="82"/>
@@ -8905,8 +8905,8 @@
       </c>
     </row>
     <row r="62" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B62" s="163"/>
-      <c r="D62" s="158" t="s">
+      <c r="B62" s="177"/>
+      <c r="D62" s="168" t="s">
         <v>110</v>
       </c>
       <c r="E62" s="79" t="s">
@@ -9008,8 +9008,8 @@
       </c>
     </row>
     <row r="63" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B63" s="163"/>
-      <c r="D63" s="159"/>
+      <c r="B63" s="177"/>
+      <c r="D63" s="169"/>
       <c r="E63" s="82" t="s">
         <v>93</v>
       </c>
@@ -9109,8 +9109,8 @@
       </c>
     </row>
     <row r="64" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B64" s="163"/>
-      <c r="D64" s="159"/>
+      <c r="B64" s="177"/>
+      <c r="D64" s="169"/>
       <c r="E64" s="83" t="s">
         <v>93</v>
       </c>
@@ -9210,8 +9210,8 @@
       </c>
     </row>
     <row r="65" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B65" s="163"/>
-      <c r="D65" s="160"/>
+      <c r="B65" s="177"/>
+      <c r="D65" s="170"/>
       <c r="E65" s="79" t="s">
         <v>98</v>
       </c>
@@ -9311,8 +9311,8 @@
       </c>
     </row>
     <row r="66" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B66" s="163"/>
-      <c r="D66" s="160"/>
+      <c r="B66" s="177"/>
+      <c r="D66" s="170"/>
       <c r="E66" s="79" t="s">
         <v>98</v>
       </c>
@@ -9412,8 +9412,8 @@
       </c>
     </row>
     <row r="67" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B67" s="163"/>
-      <c r="D67" s="160"/>
+      <c r="B67" s="177"/>
+      <c r="D67" s="170"/>
       <c r="E67" s="79" t="s">
         <v>98</v>
       </c>
@@ -9513,8 +9513,8 @@
       </c>
     </row>
     <row r="68" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B68" s="163"/>
-      <c r="D68" s="160"/>
+      <c r="B68" s="177"/>
+      <c r="D68" s="170"/>
       <c r="E68" s="79" t="s">
         <v>100</v>
       </c>
@@ -9614,8 +9614,8 @@
       </c>
     </row>
     <row r="69" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B69" s="163"/>
-      <c r="D69" s="160"/>
+      <c r="B69" s="177"/>
+      <c r="D69" s="170"/>
       <c r="E69" s="79" t="s">
         <v>100</v>
       </c>
@@ -9715,8 +9715,8 @@
       </c>
     </row>
     <row r="70" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B70" s="163"/>
-      <c r="D70" s="160"/>
+      <c r="B70" s="177"/>
+      <c r="D70" s="170"/>
       <c r="E70" s="79" t="s">
         <v>100</v>
       </c>
@@ -9816,8 +9816,8 @@
       </c>
     </row>
     <row r="71" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B71" s="163"/>
-      <c r="D71" s="160"/>
+      <c r="B71" s="177"/>
+      <c r="D71" s="170"/>
       <c r="E71" s="79" t="s">
         <v>102</v>
       </c>
@@ -9950,8 +9950,8 @@
       <c r="BV71" s="5"/>
     </row>
     <row r="72" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B72" s="163"/>
-      <c r="D72" s="160"/>
+      <c r="B72" s="177"/>
+      <c r="D72" s="170"/>
       <c r="E72" s="79" t="s">
         <v>102</v>
       </c>
@@ -10084,8 +10084,8 @@
       <c r="BV72" s="5"/>
     </row>
     <row r="73" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B73" s="163"/>
-      <c r="D73" s="160"/>
+      <c r="B73" s="177"/>
+      <c r="D73" s="170"/>
       <c r="E73" s="79" t="s">
         <v>102</v>
       </c>
@@ -10218,8 +10218,8 @@
       <c r="BV73" s="5"/>
     </row>
     <row r="74" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B74" s="163"/>
-      <c r="D74" s="160"/>
+      <c r="B74" s="177"/>
+      <c r="D74" s="170"/>
       <c r="E74" s="79" t="s">
         <v>104</v>
       </c>
@@ -10352,8 +10352,8 @@
       <c r="BV74" s="5"/>
     </row>
     <row r="75" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B75" s="163"/>
-      <c r="D75" s="160"/>
+      <c r="B75" s="177"/>
+      <c r="D75" s="170"/>
       <c r="E75" s="79" t="s">
         <v>104</v>
       </c>
@@ -10486,8 +10486,8 @@
       <c r="BV75" s="5"/>
     </row>
     <row r="76" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B76" s="163"/>
-      <c r="D76" s="160"/>
+      <c r="B76" s="177"/>
+      <c r="D76" s="170"/>
       <c r="E76" s="79" t="s">
         <v>104</v>
       </c>
@@ -10620,13 +10620,13 @@
       <c r="BV76" s="5"/>
     </row>
     <row r="77" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B77" s="163"/>
+      <c r="B77" s="177"/>
       <c r="D77" s="84"/>
       <c r="E77" s="82"/>
       <c r="F77" s="82"/>
     </row>
     <row r="78" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B78" s="163"/>
+      <c r="B78" s="177"/>
       <c r="D78" s="40"/>
       <c r="E78" s="85"/>
       <c r="F78" s="85"/>
@@ -10722,8 +10722,8 @@
       </c>
     </row>
     <row r="79" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B79" s="163"/>
-      <c r="D79" s="158" t="s">
+      <c r="B79" s="177"/>
+      <c r="D79" s="168" t="s">
         <v>111</v>
       </c>
       <c r="E79" s="79" t="s">
@@ -10825,8 +10825,8 @@
       <c r="AO79" s="1"/>
     </row>
     <row r="80" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B80" s="163"/>
-      <c r="D80" s="159"/>
+      <c r="B80" s="177"/>
+      <c r="D80" s="169"/>
       <c r="E80" s="82" t="s">
         <v>93</v>
       </c>
@@ -10926,8 +10926,8 @@
       <c r="AO80" s="1"/>
     </row>
     <row r="81" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B81" s="163"/>
-      <c r="D81" s="159"/>
+      <c r="B81" s="177"/>
+      <c r="D81" s="169"/>
       <c r="E81" s="83" t="s">
         <v>93</v>
       </c>
@@ -11027,8 +11027,8 @@
       <c r="AO81" s="1"/>
     </row>
     <row r="82" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B82" s="164"/>
-      <c r="D82" s="160"/>
+      <c r="B82" s="178"/>
+      <c r="D82" s="170"/>
       <c r="E82" s="79" t="s">
         <v>98</v>
       </c>
@@ -11127,8 +11127,8 @@
       </c>
     </row>
     <row r="83" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B83" s="164"/>
-      <c r="D83" s="160"/>
+      <c r="B83" s="178"/>
+      <c r="D83" s="170"/>
       <c r="E83" s="79" t="s">
         <v>98</v>
       </c>
@@ -11227,8 +11227,8 @@
       </c>
     </row>
     <row r="84" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B84" s="164"/>
-      <c r="D84" s="160"/>
+      <c r="B84" s="178"/>
+      <c r="D84" s="170"/>
       <c r="E84" s="79" t="s">
         <v>98</v>
       </c>
@@ -11329,8 +11329,8 @@
       <c r="AL84" s="5"/>
     </row>
     <row r="85" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B85" s="164"/>
-      <c r="D85" s="160"/>
+      <c r="B85" s="178"/>
+      <c r="D85" s="170"/>
       <c r="E85" s="79" t="s">
         <v>100</v>
       </c>
@@ -11431,8 +11431,8 @@
       <c r="AL85" s="5"/>
     </row>
     <row r="86" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B86" s="164"/>
-      <c r="D86" s="160"/>
+      <c r="B86" s="178"/>
+      <c r="D86" s="170"/>
       <c r="E86" s="79" t="s">
         <v>100</v>
       </c>
@@ -11533,8 +11533,8 @@
       <c r="AL86" s="5"/>
     </row>
     <row r="87" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B87" s="164"/>
-      <c r="D87" s="160"/>
+      <c r="B87" s="178"/>
+      <c r="D87" s="170"/>
       <c r="E87" s="79" t="s">
         <v>100</v>
       </c>
@@ -11635,8 +11635,8 @@
       <c r="AL87" s="5"/>
     </row>
     <row r="88" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B88" s="164"/>
-      <c r="D88" s="160"/>
+      <c r="B88" s="178"/>
+      <c r="D88" s="170"/>
       <c r="E88" s="79" t="s">
         <v>102</v>
       </c>
@@ -11737,8 +11737,8 @@
       <c r="AL88" s="5"/>
     </row>
     <row r="89" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B89" s="164"/>
-      <c r="D89" s="160"/>
+      <c r="B89" s="178"/>
+      <c r="D89" s="170"/>
       <c r="E89" s="79" t="s">
         <v>102</v>
       </c>
@@ -11839,8 +11839,8 @@
       <c r="AL89" s="5"/>
     </row>
     <row r="90" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B90" s="164"/>
-      <c r="D90" s="160"/>
+      <c r="B90" s="178"/>
+      <c r="D90" s="170"/>
       <c r="E90" s="79" t="s">
         <v>102</v>
       </c>
@@ -11941,8 +11941,8 @@
       <c r="AL90" s="5"/>
     </row>
     <row r="91" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B91" s="164"/>
-      <c r="D91" s="160"/>
+      <c r="B91" s="178"/>
+      <c r="D91" s="170"/>
       <c r="E91" s="79" t="s">
         <v>104</v>
       </c>
@@ -12043,8 +12043,8 @@
       <c r="AL91" s="5"/>
     </row>
     <row r="92" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B92" s="164"/>
-      <c r="D92" s="160"/>
+      <c r="B92" s="178"/>
+      <c r="D92" s="170"/>
       <c r="E92" s="79" t="s">
         <v>104</v>
       </c>
@@ -12145,8 +12145,8 @@
       <c r="AL92" s="5"/>
     </row>
     <row r="93" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B93" s="164"/>
-      <c r="D93" s="160"/>
+      <c r="B93" s="178"/>
+      <c r="D93" s="170"/>
       <c r="E93" s="79" t="s">
         <v>104</v>
       </c>
@@ -12247,10 +12247,10 @@
       <c r="AL93" s="5"/>
     </row>
     <row r="94" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B94" s="164"/>
+      <c r="B94" s="178"/>
     </row>
     <row r="95" spans="2:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="164"/>
+      <c r="B95" s="178"/>
       <c r="G95" s="1">
         <v>2021</v>
       </c>
@@ -12343,8 +12343,8 @@
       </c>
     </row>
     <row r="96" spans="2:41" x14ac:dyDescent="0.25">
-      <c r="B96" s="164"/>
-      <c r="D96" s="158" t="s">
+      <c r="B96" s="178"/>
+      <c r="D96" s="168" t="s">
         <v>112</v>
       </c>
       <c r="E96" s="79" t="s">
@@ -12445,8 +12445,8 @@
       </c>
     </row>
     <row r="97" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B97" s="164"/>
-      <c r="D97" s="159"/>
+      <c r="B97" s="178"/>
+      <c r="D97" s="169"/>
       <c r="E97" s="82" t="s">
         <v>93</v>
       </c>
@@ -12545,8 +12545,8 @@
       </c>
     </row>
     <row r="98" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B98" s="164"/>
-      <c r="D98" s="159"/>
+      <c r="B98" s="178"/>
+      <c r="D98" s="169"/>
       <c r="E98" s="83" t="s">
         <v>93</v>
       </c>
@@ -12645,8 +12645,8 @@
       </c>
     </row>
     <row r="99" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B99" s="164"/>
-      <c r="D99" s="160"/>
+      <c r="B99" s="178"/>
+      <c r="D99" s="170"/>
       <c r="E99" s="79" t="s">
         <v>98</v>
       </c>
@@ -12745,8 +12745,8 @@
       </c>
     </row>
     <row r="100" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B100" s="164"/>
-      <c r="D100" s="160"/>
+      <c r="B100" s="178"/>
+      <c r="D100" s="170"/>
       <c r="E100" s="79" t="s">
         <v>98</v>
       </c>
@@ -12845,8 +12845,8 @@
       </c>
     </row>
     <row r="101" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B101" s="164"/>
-      <c r="D101" s="160"/>
+      <c r="B101" s="178"/>
+      <c r="D101" s="170"/>
       <c r="E101" s="79" t="s">
         <v>98</v>
       </c>
@@ -12945,8 +12945,8 @@
       </c>
     </row>
     <row r="102" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B102" s="164"/>
-      <c r="D102" s="160"/>
+      <c r="B102" s="178"/>
+      <c r="D102" s="170"/>
       <c r="E102" s="79" t="s">
         <v>100</v>
       </c>
@@ -13045,8 +13045,8 @@
       </c>
     </row>
     <row r="103" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B103" s="164"/>
-      <c r="D103" s="160"/>
+      <c r="B103" s="178"/>
+      <c r="D103" s="170"/>
       <c r="E103" s="79" t="s">
         <v>100</v>
       </c>
@@ -13145,8 +13145,8 @@
       </c>
     </row>
     <row r="104" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B104" s="164"/>
-      <c r="D104" s="160"/>
+      <c r="B104" s="178"/>
+      <c r="D104" s="170"/>
       <c r="E104" s="79" t="s">
         <v>100</v>
       </c>
@@ -13245,8 +13245,8 @@
       </c>
     </row>
     <row r="105" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B105" s="164"/>
-      <c r="D105" s="160"/>
+      <c r="B105" s="178"/>
+      <c r="D105" s="170"/>
       <c r="E105" s="79" t="s">
         <v>102</v>
       </c>
@@ -13345,8 +13345,8 @@
       </c>
     </row>
     <row r="106" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B106" s="164"/>
-      <c r="D106" s="160"/>
+      <c r="B106" s="178"/>
+      <c r="D106" s="170"/>
       <c r="E106" s="79" t="s">
         <v>102</v>
       </c>
@@ -13445,8 +13445,8 @@
       </c>
     </row>
     <row r="107" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B107" s="164"/>
-      <c r="D107" s="160"/>
+      <c r="B107" s="178"/>
+      <c r="D107" s="170"/>
       <c r="E107" s="79" t="s">
         <v>102</v>
       </c>
@@ -13545,8 +13545,8 @@
       </c>
     </row>
     <row r="108" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B108" s="164"/>
-      <c r="D108" s="160"/>
+      <c r="B108" s="178"/>
+      <c r="D108" s="170"/>
       <c r="E108" s="79" t="s">
         <v>104</v>
       </c>
@@ -13645,8 +13645,8 @@
       </c>
     </row>
     <row r="109" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B109" s="164"/>
-      <c r="D109" s="160"/>
+      <c r="B109" s="178"/>
+      <c r="D109" s="170"/>
       <c r="E109" s="79" t="s">
         <v>104</v>
       </c>
@@ -13745,8 +13745,8 @@
       </c>
     </row>
     <row r="110" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B110" s="164"/>
-      <c r="D110" s="160"/>
+      <c r="B110" s="178"/>
+      <c r="D110" s="170"/>
       <c r="E110" s="79" t="s">
         <v>104</v>
       </c>
@@ -13845,10 +13845,10 @@
       </c>
     </row>
     <row r="111" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B111" s="164"/>
+      <c r="B111" s="178"/>
     </row>
     <row r="112" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B112" s="164"/>
+      <c r="B112" s="178"/>
       <c r="G112" s="1">
         <v>2021</v>
       </c>
@@ -13941,8 +13941,8 @@
       </c>
     </row>
     <row r="113" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B113" s="164"/>
-      <c r="D113" s="158" t="s">
+      <c r="B113" s="178"/>
+      <c r="D113" s="168" t="s">
         <v>113</v>
       </c>
       <c r="E113" s="79" t="s">
@@ -14044,8 +14044,8 @@
       </c>
     </row>
     <row r="114" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B114" s="164"/>
-      <c r="D114" s="159"/>
+      <c r="B114" s="178"/>
+      <c r="D114" s="169"/>
       <c r="E114" s="82" t="s">
         <v>93</v>
       </c>
@@ -14145,8 +14145,8 @@
       </c>
     </row>
     <row r="115" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B115" s="164"/>
-      <c r="D115" s="159"/>
+      <c r="B115" s="178"/>
+      <c r="D115" s="169"/>
       <c r="E115" s="83" t="s">
         <v>93</v>
       </c>
@@ -14246,8 +14246,8 @@
       </c>
     </row>
     <row r="116" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B116" s="164"/>
-      <c r="D116" s="160"/>
+      <c r="B116" s="178"/>
+      <c r="D116" s="170"/>
       <c r="E116" s="79" t="s">
         <v>98</v>
       </c>
@@ -14347,8 +14347,8 @@
       </c>
     </row>
     <row r="117" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B117" s="164"/>
-      <c r="D117" s="160"/>
+      <c r="B117" s="178"/>
+      <c r="D117" s="170"/>
       <c r="E117" s="79" t="s">
         <v>98</v>
       </c>
@@ -14448,8 +14448,8 @@
       </c>
     </row>
     <row r="118" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B118" s="164"/>
-      <c r="D118" s="160"/>
+      <c r="B118" s="178"/>
+      <c r="D118" s="170"/>
       <c r="E118" s="79" t="s">
         <v>98</v>
       </c>
@@ -14549,8 +14549,8 @@
       </c>
     </row>
     <row r="119" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B119" s="164"/>
-      <c r="D119" s="160"/>
+      <c r="B119" s="178"/>
+      <c r="D119" s="170"/>
       <c r="E119" s="79" t="s">
         <v>100</v>
       </c>
@@ -14650,8 +14650,8 @@
       </c>
     </row>
     <row r="120" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B120" s="164"/>
-      <c r="D120" s="160"/>
+      <c r="B120" s="178"/>
+      <c r="D120" s="170"/>
       <c r="E120" s="79" t="s">
         <v>100</v>
       </c>
@@ -14751,8 +14751,8 @@
       </c>
     </row>
     <row r="121" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B121" s="164"/>
-      <c r="D121" s="160"/>
+      <c r="B121" s="178"/>
+      <c r="D121" s="170"/>
       <c r="E121" s="79" t="s">
         <v>100</v>
       </c>
@@ -14852,8 +14852,8 @@
       </c>
     </row>
     <row r="122" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B122" s="164"/>
-      <c r="D122" s="160"/>
+      <c r="B122" s="178"/>
+      <c r="D122" s="170"/>
       <c r="E122" s="79" t="s">
         <v>102</v>
       </c>
@@ -14953,8 +14953,8 @@
       </c>
     </row>
     <row r="123" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B123" s="164"/>
-      <c r="D123" s="160"/>
+      <c r="B123" s="178"/>
+      <c r="D123" s="170"/>
       <c r="E123" s="79" t="s">
         <v>102</v>
       </c>
@@ -15054,8 +15054,8 @@
       </c>
     </row>
     <row r="124" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B124" s="164"/>
-      <c r="D124" s="160"/>
+      <c r="B124" s="178"/>
+      <c r="D124" s="170"/>
       <c r="E124" s="79" t="s">
         <v>102</v>
       </c>
@@ -15155,8 +15155,8 @@
       </c>
     </row>
     <row r="125" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B125" s="164"/>
-      <c r="D125" s="160"/>
+      <c r="B125" s="178"/>
+      <c r="D125" s="170"/>
       <c r="E125" s="79" t="s">
         <v>104</v>
       </c>
@@ -15256,8 +15256,8 @@
       </c>
     </row>
     <row r="126" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B126" s="164"/>
-      <c r="D126" s="160"/>
+      <c r="B126" s="178"/>
+      <c r="D126" s="170"/>
       <c r="E126" s="79" t="s">
         <v>104</v>
       </c>
@@ -15357,8 +15357,8 @@
       </c>
     </row>
     <row r="127" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B127" s="164"/>
-      <c r="D127" s="160"/>
+      <c r="B127" s="178"/>
+      <c r="D127" s="170"/>
       <c r="E127" s="79" t="s">
         <v>104</v>
       </c>
@@ -15461,23 +15461,23 @@
       <c r="B128" s="87"/>
     </row>
     <row r="129" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B129" s="162" t="s">
+      <c r="B129" s="171" t="s">
         <v>114</v>
       </c>
-      <c r="C129" s="161"/>
-      <c r="D129" s="161"/>
-      <c r="E129" s="161"/>
-      <c r="F129" s="161"/>
-      <c r="G129" s="161"/>
-      <c r="H129" s="161"/>
-      <c r="I129" s="161"/>
-      <c r="J129" s="161"/>
-      <c r="K129" s="161"/>
-      <c r="L129" s="161"/>
-      <c r="M129" s="161"/>
-      <c r="N129" s="161"/>
-      <c r="O129" s="161"/>
-      <c r="P129" s="161"/>
+      <c r="C129" s="145"/>
+      <c r="D129" s="145"/>
+      <c r="E129" s="145"/>
+      <c r="F129" s="145"/>
+      <c r="G129" s="145"/>
+      <c r="H129" s="145"/>
+      <c r="I129" s="145"/>
+      <c r="J129" s="145"/>
+      <c r="K129" s="145"/>
+      <c r="L129" s="145"/>
+      <c r="M129" s="145"/>
+      <c r="N129" s="145"/>
+      <c r="O129" s="145"/>
+      <c r="P129" s="145"/>
       <c r="Q129" s="50"/>
       <c r="R129" s="50"/>
       <c r="S129" s="50"/>
@@ -15512,21 +15512,21 @@
     </row>
     <row r="131" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B131" s="40"/>
-      <c r="C131" s="152" t="s">
+      <c r="C131" s="172" t="s">
         <v>115</v>
       </c>
-      <c r="D131" s="153"/>
-      <c r="E131" s="153"/>
-      <c r="F131" s="153"/>
-      <c r="G131" s="153"/>
-      <c r="H131" s="153"/>
-      <c r="I131" s="155" t="s">
+      <c r="D131" s="173"/>
+      <c r="E131" s="173"/>
+      <c r="F131" s="173"/>
+      <c r="G131" s="173"/>
+      <c r="H131" s="173"/>
+      <c r="I131" s="174" t="s">
         <v>116</v>
       </c>
-      <c r="J131" s="156"/>
-      <c r="K131" s="156"/>
-      <c r="L131" s="156"/>
-      <c r="M131" s="157"/>
+      <c r="J131" s="175"/>
+      <c r="K131" s="175"/>
+      <c r="L131" s="175"/>
+      <c r="M131" s="176"/>
       <c r="N131" s="89" t="s">
         <v>117</v>
       </c>
@@ -15544,14 +15544,14 @@
     </row>
     <row r="132" spans="2:28" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="40"/>
-      <c r="C132" s="142" t="s">
+      <c r="C132" s="162" t="s">
         <v>119</v>
       </c>
-      <c r="D132" s="143"/>
-      <c r="E132" s="143"/>
-      <c r="F132" s="143"/>
-      <c r="G132" s="143"/>
-      <c r="H132" s="144"/>
+      <c r="D132" s="163"/>
+      <c r="E132" s="163"/>
+      <c r="F132" s="163"/>
+      <c r="G132" s="163"/>
+      <c r="H132" s="164"/>
       <c r="I132" t="s">
         <v>95</v>
       </c>
@@ -15562,14 +15562,14 @@
     </row>
     <row r="133" spans="2:28" ht="14.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="40"/>
-      <c r="C133" s="142" t="s">
+      <c r="C133" s="162" t="s">
         <v>120</v>
       </c>
-      <c r="D133" s="143"/>
-      <c r="E133" s="143"/>
-      <c r="F133" s="143"/>
-      <c r="G133" s="143"/>
-      <c r="H133" s="144"/>
+      <c r="D133" s="163"/>
+      <c r="E133" s="163"/>
+      <c r="F133" s="163"/>
+      <c r="G133" s="163"/>
+      <c r="H133" s="164"/>
       <c r="I133" s="100" t="s">
         <v>95</v>
       </c>
@@ -15592,21 +15592,21 @@
     </row>
     <row r="134" spans="2:28" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="40"/>
-      <c r="C134" s="142" t="s">
+      <c r="C134" s="162" t="s">
         <v>109</v>
       </c>
-      <c r="D134" s="143"/>
-      <c r="E134" s="143"/>
-      <c r="F134" s="143"/>
-      <c r="G134" s="143"/>
-      <c r="H134" s="144"/>
-      <c r="I134" s="148" t="s">
+      <c r="D134" s="163"/>
+      <c r="E134" s="163"/>
+      <c r="F134" s="163"/>
+      <c r="G134" s="163"/>
+      <c r="H134" s="164"/>
+      <c r="I134" s="165" t="s">
         <v>122</v>
       </c>
-      <c r="J134" s="149"/>
-      <c r="K134" s="149"/>
-      <c r="L134" s="149"/>
-      <c r="M134" s="150"/>
+      <c r="J134" s="166"/>
+      <c r="K134" s="166"/>
+      <c r="L134" s="166"/>
+      <c r="M134" s="167"/>
       <c r="N134" s="105"/>
       <c r="O134" s="105"/>
       <c r="P134" s="106"/>
@@ -15620,21 +15620,21 @@
     </row>
     <row r="135" spans="2:28" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="40"/>
-      <c r="C135" s="142" t="s">
+      <c r="C135" s="162" t="s">
         <v>123</v>
       </c>
-      <c r="D135" s="143"/>
-      <c r="E135" s="143"/>
-      <c r="F135" s="143"/>
-      <c r="G135" s="143"/>
-      <c r="H135" s="144"/>
-      <c r="I135" s="148" t="s">
+      <c r="D135" s="163"/>
+      <c r="E135" s="163"/>
+      <c r="F135" s="163"/>
+      <c r="G135" s="163"/>
+      <c r="H135" s="164"/>
+      <c r="I135" s="165" t="s">
         <v>124</v>
       </c>
-      <c r="J135" s="149"/>
-      <c r="K135" s="149"/>
-      <c r="L135" s="149"/>
-      <c r="M135" s="150"/>
+      <c r="J135" s="166"/>
+      <c r="K135" s="166"/>
+      <c r="L135" s="166"/>
+      <c r="M135" s="167"/>
       <c r="N135" s="105"/>
       <c r="O135" s="105"/>
       <c r="P135" s="106"/>
@@ -15648,14 +15648,14 @@
     </row>
     <row r="136" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B136" s="40"/>
-      <c r="C136" s="142" t="s">
+      <c r="C136" s="162" t="s">
         <v>125</v>
       </c>
-      <c r="D136" s="143"/>
-      <c r="E136" s="143"/>
-      <c r="F136" s="143"/>
-      <c r="G136" s="143"/>
-      <c r="H136" s="144"/>
+      <c r="D136" s="163"/>
+      <c r="E136" s="163"/>
+      <c r="F136" s="163"/>
+      <c r="G136" s="163"/>
+      <c r="H136" s="164"/>
       <c r="I136" s="108" t="s">
         <v>95</v>
       </c>
@@ -15676,14 +15676,14 @@
     </row>
     <row r="137" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B137" s="40"/>
-      <c r="C137" s="145" t="s">
+      <c r="C137" s="179" t="s">
         <v>126</v>
       </c>
-      <c r="D137" s="146"/>
-      <c r="E137" s="146"/>
-      <c r="F137" s="146"/>
-      <c r="G137" s="146"/>
-      <c r="H137" s="147"/>
+      <c r="D137" s="180"/>
+      <c r="E137" s="180"/>
+      <c r="F137" s="180"/>
+      <c r="G137" s="180"/>
+      <c r="H137" s="181"/>
       <c r="I137" s="112" t="s">
         <v>95</v>
       </c>
@@ -15704,12 +15704,12 @@
     </row>
     <row r="138" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B138" s="40"/>
-      <c r="C138" s="151"/>
-      <c r="D138" s="151"/>
-      <c r="E138" s="151"/>
-      <c r="F138" s="151"/>
-      <c r="G138" s="151"/>
-      <c r="H138" s="151"/>
+      <c r="C138" s="182"/>
+      <c r="D138" s="182"/>
+      <c r="E138" s="182"/>
+      <c r="F138" s="182"/>
+      <c r="G138" s="182"/>
+      <c r="H138" s="182"/>
       <c r="I138" s="116"/>
       <c r="J138" s="116"/>
       <c r="K138" s="116"/>
@@ -15728,21 +15728,21 @@
     </row>
     <row r="139" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B139" s="40"/>
-      <c r="C139" s="152" t="s">
+      <c r="C139" s="172" t="s">
         <v>127</v>
       </c>
-      <c r="D139" s="153"/>
-      <c r="E139" s="153"/>
-      <c r="F139" s="153"/>
-      <c r="G139" s="153"/>
-      <c r="H139" s="154"/>
-      <c r="I139" s="155" t="s">
+      <c r="D139" s="173"/>
+      <c r="E139" s="173"/>
+      <c r="F139" s="173"/>
+      <c r="G139" s="173"/>
+      <c r="H139" s="183"/>
+      <c r="I139" s="174" t="s">
         <v>116</v>
       </c>
-      <c r="J139" s="156"/>
-      <c r="K139" s="156"/>
-      <c r="L139" s="156"/>
-      <c r="M139" s="157"/>
+      <c r="J139" s="175"/>
+      <c r="K139" s="175"/>
+      <c r="L139" s="175"/>
+      <c r="M139" s="176"/>
       <c r="N139" s="89" t="s">
         <v>117</v>
       </c>
@@ -15760,14 +15760,14 @@
     </row>
     <row r="140" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B140" s="40"/>
-      <c r="C140" s="142" t="s">
+      <c r="C140" s="162" t="s">
         <v>120</v>
       </c>
-      <c r="D140" s="143"/>
-      <c r="E140" s="143"/>
-      <c r="F140" s="143"/>
-      <c r="G140" s="143"/>
-      <c r="H140" s="144"/>
+      <c r="D140" s="163"/>
+      <c r="E140" s="163"/>
+      <c r="F140" s="163"/>
+      <c r="G140" s="163"/>
+      <c r="H140" s="164"/>
       <c r="I140" s="100" t="s">
         <v>95</v>
       </c>
@@ -15851,14 +15851,14 @@
     </row>
     <row r="143" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B143" s="40"/>
-      <c r="C143" s="142" t="s">
+      <c r="C143" s="162" t="s">
         <v>123</v>
       </c>
-      <c r="D143" s="143"/>
-      <c r="E143" s="143"/>
-      <c r="F143" s="143"/>
-      <c r="G143" s="143"/>
-      <c r="H143" s="144"/>
+      <c r="D143" s="163"/>
+      <c r="E143" s="163"/>
+      <c r="F143" s="163"/>
+      <c r="G143" s="163"/>
+      <c r="H143" s="164"/>
       <c r="I143" s="122" t="s">
         <v>128</v>
       </c>
@@ -15879,14 +15879,14 @@
     </row>
     <row r="144" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B144" s="40"/>
-      <c r="C144" s="142" t="s">
+      <c r="C144" s="162" t="s">
         <v>125</v>
       </c>
-      <c r="D144" s="143"/>
-      <c r="E144" s="143"/>
-      <c r="F144" s="143"/>
-      <c r="G144" s="143"/>
-      <c r="H144" s="144"/>
+      <c r="D144" s="163"/>
+      <c r="E144" s="163"/>
+      <c r="F144" s="163"/>
+      <c r="G144" s="163"/>
+      <c r="H144" s="164"/>
       <c r="I144" s="122" t="s">
         <v>128</v>
       </c>
@@ -15907,14 +15907,14 @@
     </row>
     <row r="145" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B145" s="40"/>
-      <c r="C145" s="145" t="s">
+      <c r="C145" s="179" t="s">
         <v>131</v>
       </c>
-      <c r="D145" s="146"/>
-      <c r="E145" s="146"/>
-      <c r="F145" s="146"/>
-      <c r="G145" s="146"/>
-      <c r="H145" s="147"/>
+      <c r="D145" s="180"/>
+      <c r="E145" s="180"/>
+      <c r="F145" s="180"/>
+      <c r="G145" s="180"/>
+      <c r="H145" s="181"/>
       <c r="I145" s="112" t="s">
         <v>95</v>
       </c>
@@ -16166,16 +16166,17 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="C7:Q7"/>
-    <mergeCell ref="B9:B36"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:L9"/>
-    <mergeCell ref="D11:L11"/>
-    <mergeCell ref="D12:L12"/>
-    <mergeCell ref="D13:L13"/>
-    <mergeCell ref="C15:P16"/>
+    <mergeCell ref="C140:H140"/>
+    <mergeCell ref="C143:H143"/>
+    <mergeCell ref="C144:H144"/>
+    <mergeCell ref="C145:H145"/>
+    <mergeCell ref="C135:H135"/>
+    <mergeCell ref="I135:M135"/>
+    <mergeCell ref="C136:H136"/>
+    <mergeCell ref="C137:H137"/>
+    <mergeCell ref="C138:H138"/>
+    <mergeCell ref="C139:H139"/>
+    <mergeCell ref="I139:M139"/>
     <mergeCell ref="C134:H134"/>
     <mergeCell ref="I134:M134"/>
     <mergeCell ref="D17:D27"/>
@@ -16192,17 +16193,16 @@
     <mergeCell ref="D79:D93"/>
     <mergeCell ref="D96:D110"/>
     <mergeCell ref="D113:D127"/>
-    <mergeCell ref="I135:M135"/>
-    <mergeCell ref="C136:H136"/>
-    <mergeCell ref="C137:H137"/>
-    <mergeCell ref="C138:H138"/>
-    <mergeCell ref="C139:H139"/>
-    <mergeCell ref="I139:M139"/>
-    <mergeCell ref="C140:H140"/>
-    <mergeCell ref="C143:H143"/>
-    <mergeCell ref="C144:H144"/>
-    <mergeCell ref="C145:H145"/>
-    <mergeCell ref="C135:H135"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="C7:Q7"/>
+    <mergeCell ref="B9:B36"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:L9"/>
+    <mergeCell ref="D11:L11"/>
+    <mergeCell ref="D12:L12"/>
+    <mergeCell ref="D13:L13"/>
+    <mergeCell ref="C15:P16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M1" r:id="rId1" display="https://atb.nrel.gov/electricity/2022/utility-scale_battery_storage" xr:uid="{7816EC9A-0454-4087-A6E1-F971C99AA20E}"/>
@@ -17060,17 +17060,17 @@
   <dimension ref="A1:AE12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AE2"/>
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="47" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B1">
         <v>2021</v>
@@ -17165,7 +17165,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2">
         <v>272875</v>
@@ -17177,85 +17177,85 @@
         <v>303546</v>
       </c>
       <c r="E2">
-        <v>277345</v>
+        <v>275720</v>
       </c>
       <c r="F2">
-        <v>256728</v>
+        <v>254008</v>
       </c>
       <c r="G2">
-        <v>240275</v>
+        <v>237399</v>
       </c>
       <c r="H2">
-        <v>226464</v>
+        <v>223663</v>
       </c>
       <c r="I2">
-        <v>214618</v>
+        <v>212018</v>
       </c>
       <c r="J2">
-        <v>204553</v>
+        <v>202332</v>
       </c>
       <c r="K2">
-        <v>196075</v>
+        <v>194107</v>
       </c>
       <c r="L2">
-        <v>188655</v>
+        <v>186872</v>
       </c>
       <c r="M2">
-        <v>182183</v>
+        <v>180500</v>
       </c>
       <c r="N2">
-        <v>176401</v>
+        <v>174745</v>
       </c>
       <c r="O2">
-        <v>171611</v>
+        <v>169959</v>
       </c>
       <c r="P2">
-        <v>167430</v>
+        <v>165780</v>
       </c>
       <c r="Q2">
-        <v>163809</v>
+        <v>162166</v>
       </c>
       <c r="R2">
-        <v>160633</v>
+        <v>159002</v>
       </c>
       <c r="S2">
-        <v>157780</v>
+        <v>156172</v>
       </c>
       <c r="T2">
-        <v>155218</v>
+        <v>153632</v>
       </c>
       <c r="U2">
-        <v>152921</v>
+        <v>151363</v>
       </c>
       <c r="V2">
-        <v>150890</v>
+        <v>149361</v>
       </c>
       <c r="W2">
-        <v>149018</v>
+        <v>147535</v>
       </c>
       <c r="X2">
-        <v>147310</v>
+        <v>145853</v>
       </c>
       <c r="Y2">
-        <v>145744</v>
+        <v>144309</v>
       </c>
       <c r="Z2">
-        <v>144287</v>
+        <v>142883</v>
       </c>
       <c r="AA2">
-        <v>142963</v>
+        <v>141583</v>
       </c>
       <c r="AB2">
-        <v>141726</v>
+        <v>140367</v>
       </c>
       <c r="AC2">
-        <v>140576</v>
+        <v>139237</v>
       </c>
       <c r="AD2">
-        <v>139495</v>
+        <v>138175</v>
       </c>
       <c r="AE2">
-        <v>138485</v>
+        <v>137182</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -17378,7 +17378,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B5">
         <v>2021</v>
@@ -17473,7 +17473,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B6">
         <v>253384</v>

</xml_diff>